<commit_message>
dataloggin working, but some variables missing change block size from word to something larger
</commit_message>
<xml_diff>
--- a/tables/nomenclature/tags.xlsx
+++ b/tables/nomenclature/tags.xlsx
@@ -5,33 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Accacio\Documents\docsTCC\tables\nomenclature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCA5\Documents\Accacio\docsTCC\tables\nomenclature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C53B88-4A40-47EB-8B08-72EA2A5F1F94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF571C07-1F5B-4D86-81E8-684379DD1196}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11385" xr2:uid="{5B2C9D61-D82C-476D-A610-2CB6D10DBD6E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5B2C9D61-D82C-476D-A610-2CB6D10DBD6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="264">
   <si>
     <t xml:space="preserve">I_MAG1EXT </t>
   </si>
@@ -81,9 +75,6 @@
     <t xml:space="preserve">I_RDCRET  </t>
   </si>
   <si>
-    <t xml:space="preserve">I_PSP     </t>
-  </si>
-  <si>
     <t xml:space="preserve">I_METAL   </t>
   </si>
   <si>
@@ -424,6 +415,408 @@
   </si>
   <si>
     <t>I_SUHE</t>
+  </si>
+  <si>
+    <t>IOVEC</t>
+  </si>
+  <si>
+    <t>'I_MAG1EXT'</t>
+  </si>
+  <si>
+    <t>'I_MAG1RET'</t>
+  </si>
+  <si>
+    <t>'I_MAG1EMPT'</t>
+  </si>
+  <si>
+    <t>'I_MAG2EXT'</t>
+  </si>
+  <si>
+    <t>'I_MAG2RET'</t>
+  </si>
+  <si>
+    <t>'I_MAG2EMPT'</t>
+  </si>
+  <si>
+    <t>'I_PSLD'</t>
+  </si>
+  <si>
+    <t>'I_PSCD'</t>
+  </si>
+  <si>
+    <t>'I_PSRD'</t>
+  </si>
+  <si>
+    <t>'I_RELAY1'</t>
+  </si>
+  <si>
+    <t>'I_LDCEXT'</t>
+  </si>
+  <si>
+    <t>'I_LDCRET'</t>
+  </si>
+  <si>
+    <t>'I_CDCEXT'</t>
+  </si>
+  <si>
+    <t>'I_CDCRET'</t>
+  </si>
+  <si>
+    <t>'I_RDCEXT'</t>
+  </si>
+  <si>
+    <t>'I_RDCRET'</t>
+  </si>
+  <si>
+    <t>'I_METAL'</t>
+  </si>
+  <si>
+    <t>'I_PSEOC'</t>
+  </si>
+  <si>
+    <t>'O_MAG1EXT'</t>
+  </si>
+  <si>
+    <t>'O_MAG1RET'</t>
+  </si>
+  <si>
+    <t>'O_MAG2EXT'</t>
+  </si>
+  <si>
+    <t>'O_MAG2RET'</t>
+  </si>
+  <si>
+    <t>'O_RDCEXT'</t>
+  </si>
+  <si>
+    <t>'O_CDCEXT'</t>
+  </si>
+  <si>
+    <t>'O_LDCEXT'</t>
+  </si>
+  <si>
+    <t>'O_CBFW'</t>
+  </si>
+  <si>
+    <t>'O_CBREV'</t>
+  </si>
+  <si>
+    <t>'I_SDO'</t>
+  </si>
+  <si>
+    <t>'I_SDC'</t>
+  </si>
+  <si>
+    <t>'I_AUHEXT'</t>
+  </si>
+  <si>
+    <t>'I_AUHRET'</t>
+  </si>
+  <si>
+    <t>'I_INDARM'</t>
+  </si>
+  <si>
+    <t>'I_ARMLOW'</t>
+  </si>
+  <si>
+    <t>'I_ARMHIG'</t>
+  </si>
+  <si>
+    <t>'I_ARMRET'</t>
+  </si>
+  <si>
+    <t>'I_ARMEXT'</t>
+  </si>
+  <si>
+    <t>'I_SUVE'</t>
+  </si>
+  <si>
+    <t>'I_SUILS'</t>
+  </si>
+  <si>
+    <t>'I_SUSLS'</t>
+  </si>
+  <si>
+    <t>'I_SUEXT'</t>
+  </si>
+  <si>
+    <t>'I_SURET'</t>
+  </si>
+  <si>
+    <t>'I_RELAY2'</t>
+  </si>
+  <si>
+    <t>'I_SUHE'</t>
+  </si>
+  <si>
+    <t>'I_SURLS'</t>
+  </si>
+  <si>
+    <t>'I_SULLS'</t>
+  </si>
+  <si>
+    <t>'I_SUARMALE'</t>
+  </si>
+  <si>
+    <t>'O_SDO'</t>
+  </si>
+  <si>
+    <t>'O_SDC'</t>
+  </si>
+  <si>
+    <t>'O_AUHRET'</t>
+  </si>
+  <si>
+    <t>'O_AUHEXT'</t>
+  </si>
+  <si>
+    <t>'O_PRESSLOW'</t>
+  </si>
+  <si>
+    <t>'O_PRESSHIG'</t>
+  </si>
+  <si>
+    <t>'O_ARMHIG'</t>
+  </si>
+  <si>
+    <t>'O_VACON'</t>
+  </si>
+  <si>
+    <t>'O_ARMEXT'</t>
+  </si>
+  <si>
+    <t>'O_ARMCCW'</t>
+  </si>
+  <si>
+    <t>'O_ARMCW'</t>
+  </si>
+  <si>
+    <t>'O_SUEXT'</t>
+  </si>
+  <si>
+    <t>'O_SUUP'</t>
+  </si>
+  <si>
+    <t>'O_SUDWN'</t>
+  </si>
+  <si>
+    <t>'O_SURIGHT'</t>
+  </si>
+  <si>
+    <t>'O_SULEFT'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I_WHIT  </t>
+  </si>
+  <si>
+    <t>ConcUP</t>
+  </si>
+  <si>
+    <t>ConcDWN</t>
+  </si>
+  <si>
+    <t>'I_WHIT'</t>
+  </si>
+  <si>
+    <t>'ConcDWN'</t>
+  </si>
+  <si>
+    <t>'ConcUP'</t>
+  </si>
+  <si>
+    <t>'0'</t>
+  </si>
+  <si>
+    <t>'1'</t>
+  </si>
+  <si>
+    <t>'2'</t>
+  </si>
+  <si>
+    <t>'3'</t>
+  </si>
+  <si>
+    <t>'4'</t>
+  </si>
+  <si>
+    <t>'5'</t>
+  </si>
+  <si>
+    <t>'6'</t>
+  </si>
+  <si>
+    <t>'7'</t>
+  </si>
+  <si>
+    <t>'8'</t>
+  </si>
+  <si>
+    <t>'9'</t>
+  </si>
+  <si>
+    <t>'10'</t>
+  </si>
+  <si>
+    <t>'11'</t>
+  </si>
+  <si>
+    <t>'12'</t>
+  </si>
+  <si>
+    <t>'13'</t>
+  </si>
+  <si>
+    <t>'14'</t>
+  </si>
+  <si>
+    <t>'15'</t>
+  </si>
+  <si>
+    <t>'16'</t>
+  </si>
+  <si>
+    <t>'17'</t>
+  </si>
+  <si>
+    <t>'18'</t>
+  </si>
+  <si>
+    <t>'19'</t>
+  </si>
+  <si>
+    <t>'20'</t>
+  </si>
+  <si>
+    <t>'21'</t>
+  </si>
+  <si>
+    <t>'22'</t>
+  </si>
+  <si>
+    <t>'23'</t>
+  </si>
+  <si>
+    <t>'24'</t>
+  </si>
+  <si>
+    <t>'25'</t>
+  </si>
+  <si>
+    <t>'26'</t>
+  </si>
+  <si>
+    <t>'27'</t>
+  </si>
+  <si>
+    <t>'28'</t>
+  </si>
+  <si>
+    <t>'29'</t>
+  </si>
+  <si>
+    <t>'30'</t>
+  </si>
+  <si>
+    <t>'31'</t>
+  </si>
+  <si>
+    <t>'32'</t>
+  </si>
+  <si>
+    <t>'33'</t>
+  </si>
+  <si>
+    <t>'34'</t>
+  </si>
+  <si>
+    <t>'35'</t>
+  </si>
+  <si>
+    <t>'36'</t>
+  </si>
+  <si>
+    <t>'37'</t>
+  </si>
+  <si>
+    <t>'38'</t>
+  </si>
+  <si>
+    <t>'39'</t>
+  </si>
+  <si>
+    <t>'40'</t>
+  </si>
+  <si>
+    <t>'41'</t>
+  </si>
+  <si>
+    <t>'42'</t>
+  </si>
+  <si>
+    <t>'43'</t>
+  </si>
+  <si>
+    <t>'44'</t>
+  </si>
+  <si>
+    <t>'45'</t>
+  </si>
+  <si>
+    <t>'46'</t>
+  </si>
+  <si>
+    <t>'47'</t>
+  </si>
+  <si>
+    <t>'48'</t>
+  </si>
+  <si>
+    <t>'49'</t>
+  </si>
+  <si>
+    <t>'50'</t>
+  </si>
+  <si>
+    <t>'51'</t>
+  </si>
+  <si>
+    <t>'52'</t>
+  </si>
+  <si>
+    <t>'53'</t>
+  </si>
+  <si>
+    <t>'54'</t>
+  </si>
+  <si>
+    <t>'55'</t>
+  </si>
+  <si>
+    <t>'56'</t>
+  </si>
+  <si>
+    <t>'57'</t>
+  </si>
+  <si>
+    <t>'58'</t>
+  </si>
+  <si>
+    <t>'59'</t>
+  </si>
+  <si>
+    <t>'60'</t>
+  </si>
+  <si>
+    <t>'61'</t>
+  </si>
+  <si>
+    <t>'62'</t>
+  </si>
+  <si>
+    <t>'63'</t>
+  </si>
+  <si>
+    <t>'64'</t>
   </si>
 </sst>
 </file>
@@ -778,493 +1171,1336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9E0FC4-89B6-46D6-A6A3-B8909DFBC4FA}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32:K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
       <c r="G2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" t="s">
         <v>125</v>
       </c>
-      <c r="H2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>132</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>135</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="K7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>136</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
+        <v>137</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="K9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>138</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>139</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="K11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
+        <v>140</v>
+      </c>
+      <c r="M11">
+        <v>9</v>
+      </c>
+      <c r="N11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="K12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M13">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" t="s">
+        <v>143</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>144</v>
+      </c>
+      <c r="M15">
+        <v>13</v>
+      </c>
+      <c r="N15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
+        <v>145</v>
+      </c>
+      <c r="M16">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" t="s">
+        <v>146</v>
+      </c>
+      <c r="M17">
+        <v>15</v>
+      </c>
+      <c r="N17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K18" t="s">
+        <v>193</v>
+      </c>
+      <c r="L18" t="s">
+        <v>196</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
+      </c>
+      <c r="N18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="G18" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="K19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="L19" t="s">
+        <v>147</v>
+      </c>
+      <c r="M19">
+        <v>17</v>
+      </c>
+      <c r="N19" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>92</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="K20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
+      <c r="L20" t="s">
+        <v>148</v>
+      </c>
+      <c r="M20">
+        <v>18</v>
+      </c>
+      <c r="N20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
         <v>37</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" t="s">
+        <v>75</v>
+      </c>
+      <c r="K21" t="s">
+        <v>195</v>
+      </c>
+      <c r="L21" t="s">
+        <v>197</v>
+      </c>
+      <c r="M21">
+        <v>19</v>
+      </c>
+      <c r="N21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" t="s">
         <v>93</v>
       </c>
-      <c r="H20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="K22" t="s">
+        <v>194</v>
+      </c>
+      <c r="L22" t="s">
+        <v>198</v>
+      </c>
+      <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" t="s">
+        <v>94</v>
+      </c>
+      <c r="K23" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" t="s">
+        <v>149</v>
+      </c>
+      <c r="M23">
+        <v>21</v>
+      </c>
+      <c r="N23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" t="s">
+        <v>95</v>
+      </c>
+      <c r="K24" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" t="s">
+        <v>150</v>
+      </c>
+      <c r="M24">
+        <v>22</v>
+      </c>
+      <c r="N24" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" t="s">
+        <v>111</v>
+      </c>
+      <c r="H25" t="s">
+        <v>96</v>
+      </c>
+      <c r="K25" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" t="s">
+        <v>151</v>
+      </c>
+      <c r="M25">
+        <v>23</v>
+      </c>
+      <c r="N25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" t="s">
+        <v>97</v>
+      </c>
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26" t="s">
+        <v>152</v>
+      </c>
+      <c r="M26">
+        <v>24</v>
+      </c>
+      <c r="N26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27" t="s">
+        <v>153</v>
+      </c>
+      <c r="M27">
+        <v>25</v>
+      </c>
+      <c r="N27" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" t="s">
+        <v>114</v>
+      </c>
+      <c r="H28" t="s">
+        <v>95</v>
+      </c>
+      <c r="K28" t="s">
+        <v>53</v>
+      </c>
+      <c r="L28" t="s">
+        <v>154</v>
+      </c>
+      <c r="M28">
+        <v>26</v>
+      </c>
+      <c r="N28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" t="s">
+        <v>115</v>
+      </c>
+      <c r="H29" t="s">
+        <v>99</v>
+      </c>
+      <c r="K29" t="s">
+        <v>54</v>
+      </c>
+      <c r="L29" t="s">
+        <v>155</v>
+      </c>
+      <c r="M29">
+        <v>27</v>
+      </c>
+      <c r="N29" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" t="s">
+        <v>116</v>
+      </c>
+      <c r="H30" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" t="s">
+        <v>55</v>
+      </c>
+      <c r="L30" t="s">
+        <v>156</v>
+      </c>
+      <c r="M30">
+        <v>28</v>
+      </c>
+      <c r="N30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" t="s">
+        <v>101</v>
+      </c>
+      <c r="K31" t="s">
+        <v>56</v>
+      </c>
+      <c r="L31" t="s">
+        <v>157</v>
+      </c>
+      <c r="M31">
+        <v>29</v>
+      </c>
+      <c r="N31" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" t="s">
+        <v>102</v>
+      </c>
+      <c r="K32" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" t="s">
+        <v>158</v>
+      </c>
+      <c r="M32">
+        <v>30</v>
+      </c>
+      <c r="N32" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>119</v>
+      </c>
+      <c r="H33" t="s">
+        <v>103</v>
+      </c>
+      <c r="K33" t="s">
+        <v>77</v>
+      </c>
+      <c r="L33" t="s">
+        <v>159</v>
+      </c>
+      <c r="M33">
+        <v>31</v>
+      </c>
+      <c r="N33" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>120</v>
+      </c>
+      <c r="H34" t="s">
+        <v>104</v>
+      </c>
+      <c r="K34" t="s">
+        <v>78</v>
+      </c>
+      <c r="L34" t="s">
+        <v>160</v>
+      </c>
+      <c r="M34">
+        <v>32</v>
+      </c>
+      <c r="N34" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>121</v>
+      </c>
+      <c r="H35" t="s">
+        <v>105</v>
+      </c>
+      <c r="K35" t="s">
+        <v>79</v>
+      </c>
+      <c r="L35" t="s">
+        <v>161</v>
+      </c>
+      <c r="M35">
+        <v>33</v>
+      </c>
+      <c r="N35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" t="s">
+        <v>106</v>
+      </c>
+      <c r="K36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L36" t="s">
+        <v>162</v>
+      </c>
+      <c r="M36">
+        <v>34</v>
+      </c>
+      <c r="N36" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37" t="s">
+        <v>107</v>
+      </c>
+      <c r="K37" t="s">
+        <v>81</v>
+      </c>
+      <c r="L37" t="s">
+        <v>163</v>
+      </c>
+      <c r="M37">
+        <v>35</v>
+      </c>
+      <c r="N37" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>82</v>
+      </c>
+      <c r="L38" t="s">
+        <v>164</v>
+      </c>
+      <c r="M38">
+        <v>36</v>
+      </c>
+      <c r="N38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>83</v>
+      </c>
+      <c r="L39" t="s">
+        <v>165</v>
+      </c>
+      <c r="M39">
+        <v>37</v>
+      </c>
+      <c r="N39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>84</v>
+      </c>
+      <c r="L40" t="s">
+        <v>166</v>
+      </c>
+      <c r="M40">
         <v>38</v>
       </c>
-      <c r="G21" t="s">
+      <c r="N40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>85</v>
+      </c>
+      <c r="L41" t="s">
+        <v>167</v>
+      </c>
+      <c r="M41">
+        <v>39</v>
+      </c>
+      <c r="N41" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="42" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>86</v>
+      </c>
+      <c r="L42" t="s">
+        <v>168</v>
+      </c>
+      <c r="M42">
+        <v>40</v>
+      </c>
+      <c r="N42" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>87</v>
+      </c>
+      <c r="L43" t="s">
+        <v>169</v>
+      </c>
+      <c r="M43">
+        <v>41</v>
+      </c>
+      <c r="N43" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="44" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>88</v>
+      </c>
+      <c r="L44" t="s">
+        <v>170</v>
+      </c>
+      <c r="M44">
+        <v>42</v>
+      </c>
+      <c r="N44" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>89</v>
+      </c>
+      <c r="L45" t="s">
+        <v>171</v>
+      </c>
+      <c r="M45">
+        <v>43</v>
+      </c>
+      <c r="N45" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>90</v>
+      </c>
+      <c r="L46" t="s">
+        <v>172</v>
+      </c>
+      <c r="M46">
+        <v>44</v>
+      </c>
+      <c r="N46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
         <v>129</v>
       </c>
-      <c r="H21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="L47" t="s">
+        <v>173</v>
+      </c>
+      <c r="M47">
+        <v>45</v>
+      </c>
+      <c r="N47" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>91</v>
+      </c>
+      <c r="L48" t="s">
+        <v>174</v>
+      </c>
+      <c r="M48">
+        <v>46</v>
+      </c>
+      <c r="N48" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>92</v>
+      </c>
+      <c r="L49" t="s">
+        <v>175</v>
+      </c>
+      <c r="M49">
+        <v>47</v>
+      </c>
+      <c r="N49" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>128</v>
+      </c>
+      <c r="L50" t="s">
+        <v>176</v>
+      </c>
+      <c r="M50">
+        <v>48</v>
+      </c>
+      <c r="N50" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>108</v>
+      </c>
+      <c r="L51" t="s">
+        <v>177</v>
+      </c>
+      <c r="M51">
+        <v>49</v>
+      </c>
+      <c r="N51" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
         <v>109</v>
       </c>
-      <c r="H22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="L52" t="s">
+        <v>178</v>
+      </c>
+      <c r="M52">
+        <v>50</v>
+      </c>
+      <c r="N52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
         <v>110</v>
       </c>
-      <c r="H23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="L53" t="s">
+        <v>179</v>
+      </c>
+      <c r="M53">
+        <v>51</v>
+      </c>
+      <c r="N53" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
         <v>111</v>
       </c>
-      <c r="H24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="L54" t="s">
+        <v>180</v>
+      </c>
+      <c r="M54">
+        <v>52</v>
+      </c>
+      <c r="N54" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
         <v>112</v>
       </c>
-      <c r="H25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="L55" t="s">
+        <v>181</v>
+      </c>
+      <c r="M55">
+        <v>53</v>
+      </c>
+      <c r="N55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
         <v>113</v>
       </c>
-      <c r="H26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="L56" t="s">
+        <v>182</v>
+      </c>
+      <c r="M56">
+        <v>54</v>
+      </c>
+      <c r="N56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
         <v>114</v>
       </c>
-      <c r="H27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="L57" t="s">
+        <v>183</v>
+      </c>
+      <c r="M57">
+        <v>55</v>
+      </c>
+      <c r="N57" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
         <v>115</v>
       </c>
-      <c r="H28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="L58" t="s">
+        <v>184</v>
+      </c>
+      <c r="M58">
+        <v>56</v>
+      </c>
+      <c r="N58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
         <v>116</v>
       </c>
-      <c r="H29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="L59" t="s">
+        <v>185</v>
+      </c>
+      <c r="M59">
+        <v>57</v>
+      </c>
+      <c r="N59" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K60" t="s">
         <v>117</v>
       </c>
-      <c r="H30" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="L60" t="s">
+        <v>186</v>
+      </c>
+      <c r="M60">
+        <v>58</v>
+      </c>
+      <c r="N60" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K61" t="s">
         <v>118</v>
       </c>
-      <c r="H31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G32" t="s">
+      <c r="L61" t="s">
+        <v>187</v>
+      </c>
+      <c r="M61">
+        <v>59</v>
+      </c>
+      <c r="N61" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K62" t="s">
         <v>119</v>
       </c>
-      <c r="H32" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G33" t="s">
+      <c r="L62" t="s">
+        <v>188</v>
+      </c>
+      <c r="M62">
+        <v>60</v>
+      </c>
+      <c r="N62" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="63" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K63" t="s">
         <v>120</v>
       </c>
-      <c r="H33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G34" t="s">
+      <c r="L63" t="s">
+        <v>189</v>
+      </c>
+      <c r="M63">
+        <v>61</v>
+      </c>
+      <c r="N63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="64" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
         <v>121</v>
       </c>
-      <c r="H34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G35" t="s">
+      <c r="L64" t="s">
+        <v>190</v>
+      </c>
+      <c r="M64">
+        <v>62</v>
+      </c>
+      <c r="N64" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K65" t="s">
         <v>122</v>
       </c>
-      <c r="H35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G36" t="s">
+      <c r="L65" t="s">
+        <v>191</v>
+      </c>
+      <c r="M65">
+        <v>63</v>
+      </c>
+      <c r="N65" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="66" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
         <v>123</v>
       </c>
-      <c r="H36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G37" t="s">
-        <v>124</v>
-      </c>
-      <c r="H37" t="s">
-        <v>108</v>
+      <c r="L66" t="s">
+        <v>192</v>
+      </c>
+      <c r="M66">
+        <v>64</v>
+      </c>
+      <c r="N66" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>